<commit_message>
use dropdown values in example
</commit_message>
<xml_diff>
--- a/example_tables/ENA_excel_example_ERC000033.xlsx
+++ b/example_tables/ENA_excel_example_ERC000033.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="677">
   <si>
     <t xml:space="preserve">alias</t>
   </si>
@@ -769,7 +769,7 @@
     <t xml:space="preserve">ENA_TEST1.R1.fastq.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">FASTQ</t>
+    <t xml:space="preserve">fastq</t>
   </si>
   <si>
     <t xml:space="preserve">r_20221007_030</t>
@@ -791,9 +791,6 @@
   </si>
   <si>
     <t xml:space="preserve">sff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fastq</t>
   </si>
   <si>
     <t xml:space="preserve">fasta</t>
@@ -2204,7 +2201,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="1" style="0" width="15.71"/>
   </cols>
@@ -2579,7 +2576,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="0" t="s">
@@ -2678,7 +2675,7 @@
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="1" style="0" width="15.71"/>
   </cols>
@@ -3650,7 +3647,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G1" s="0" t="s">
@@ -4327,11 +4324,11 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="1" style="0" width="15.71"/>
   </cols>
@@ -4722,7 +4719,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
@@ -4741,107 +4738,107 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4862,11 +4859,11 @@
   </sheetPr>
   <dimension ref="A1:AN101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AC17" activeCellId="0" sqref="AC17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="1" style="0" width="15.71"/>
   </cols>
@@ -4879,118 +4876,118 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4998,121 +4995,121 @@
         <v>235</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5120,19 +5117,19 @@
         <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5141,34 +5138,34 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P3" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="S3" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="T3" s="0" t="s">
         <v>352</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>353</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>50</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y3" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="AA3" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AB3" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AG3" s="0" t="s">
         <v>357</v>
-      </c>
-      <c r="AG3" s="0" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5176,19 +5173,19 @@
         <v>66</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>43916</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5197,34 +5194,34 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P4" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="S4" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="S4" s="0" t="s">
-        <v>352</v>
-      </c>
       <c r="T4" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>46</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y4" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="AA4" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="AB4" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="AB4" s="0" t="s">
-        <v>357</v>
-      </c>
       <c r="AG4" s="0" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5232,19 +5229,19 @@
         <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>43916</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5253,34 +5250,34 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P5" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="S5" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="S5" s="0" t="s">
-        <v>352</v>
-      </c>
       <c r="T5" s="0" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="U5" s="0" t="n">
         <v>70</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="W5" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="AG5" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="AB5" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="AG5" s="0" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5288,19 +5285,19 @@
         <v>70</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>43916</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5309,31 +5306,31 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P6" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="S6" s="0" t="s">
-        <v>352</v>
-      </c>
       <c r="T6" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="AG6" s="0" t="s">
         <v>367</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="Y6" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="AA6" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="AB6" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="AG6" s="0" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5867,78 +5864,78 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I1" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="M1" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="W1" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="AI1" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="W1" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AM1" s="0" t="s">
         <v>374</v>
-      </c>
-      <c r="AM1" s="0" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I2" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="M2" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>379</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="AI2" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="AI2" s="0" t="s">
+      <c r="AM2" s="0" t="s">
         <v>382</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M3" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="W3" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="AI3" s="0" t="s">
         <v>387</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>388</v>
       </c>
       <c r="AM3" s="0" t="s">
         <v>176</v>
@@ -5946,36 +5943,36 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M4" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q4" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="V4" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="W4" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="AI4" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="W4" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="AI4" s="0" t="s">
+      <c r="AM4" s="0" t="s">
         <v>392</v>
-      </c>
-      <c r="AM4" s="0" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M5" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q5" s="0" t="s">
         <v>176</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AI5" s="0" t="s">
         <v>176</v>
@@ -5983,126 +5980,126 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M6" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q6" s="0" t="s">
         <v>396</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="V6" s="0" t="s">
         <v>397</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="W6" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="AI6" s="0" t="s">
         <v>398</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="AI6" s="0" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M7" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="V7" s="0" t="s">
         <v>401</v>
       </c>
-      <c r="V7" s="0" t="s">
+      <c r="W7" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="AI7" s="0" t="s">
         <v>402</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="AI7" s="0" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M8" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="V8" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="V8" s="0" t="s">
-        <v>405</v>
-      </c>
       <c r="W8" s="0" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M9" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="V9" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="V9" s="0" t="s">
-        <v>407</v>
-      </c>
       <c r="W9" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M10" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="V10" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="V10" s="0" t="s">
-        <v>409</v>
-      </c>
       <c r="W10" s="0" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M11" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="V11" s="0" t="s">
         <v>410</v>
       </c>
-      <c r="V11" s="0" t="s">
-        <v>411</v>
-      </c>
       <c r="W11" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M12" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="V12" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="V12" s="0" t="s">
+      <c r="W12" s="0" t="s">
         <v>413</v>
-      </c>
-      <c r="W12" s="0" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M13" s="0" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M14" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="V14" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="V14" s="0" t="s">
-        <v>417</v>
-      </c>
       <c r="W14" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M15" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M16" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="W16" s="0" t="s">
         <v>176</v>
@@ -6110,1360 +6107,1360 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M18" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M19" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M20" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M21" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M22" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M23" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M24" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M25" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M26" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M27" s="0" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M28" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M29" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M30" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M31" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M32" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M33" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M34" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M35" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M36" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M37" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M38" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M39" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M40" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M41" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M42" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M43" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M44" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M45" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M46" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M47" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M48" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M49" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M50" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M51" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M52" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M53" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M54" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M55" s="0" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M56" s="0" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M57" s="0" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M58" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M59" s="0" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M60" s="0" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M61" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M62" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M63" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M64" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M65" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M66" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M67" s="0" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M68" s="0" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M69" s="0" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M70" s="0" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M71" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M72" s="0" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M73" s="0" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M74" s="0" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M75" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M76" s="0" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M77" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M78" s="0" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M79" s="0" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M80" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M81" s="0" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M82" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M83" s="0" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M84" s="0" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M85" s="0" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M86" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M87" s="0" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M88" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M89" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M90" s="0" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M91" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M92" s="0" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M93" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M94" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M95" s="0" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M96" s="0" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M97" s="0" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M98" s="0" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M99" s="0" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M100" s="0" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M101" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M102" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M103" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M104" s="0" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M105" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M106" s="0" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M107" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M108" s="0" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M109" s="0" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M110" s="0" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M111" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M112" s="0" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M113" s="0" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M114" s="0" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M115" s="0" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M116" s="0" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M117" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M118" s="0" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M119" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M120" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M121" s="0" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M122" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M123" s="0" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M124" s="0" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M125" s="0" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M126" s="0" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M127" s="0" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M128" s="0" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M129" s="0" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M130" s="0" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M131" s="0" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M132" s="0" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M133" s="0" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M134" s="0" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M135" s="0" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M136" s="0" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M137" s="0" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M138" s="0" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M139" s="0" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M140" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M141" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M142" s="0" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M143" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M144" s="0" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M145" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M146" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M147" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M148" s="0" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M149" s="0" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M150" s="0" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M151" s="0" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M152" s="0" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M153" s="0" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M154" s="0" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M155" s="0" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M156" s="0" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M157" s="0" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M158" s="0" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M159" s="0" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M160" s="0" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M161" s="0" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M162" s="0" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M163" s="0" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M164" s="0" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M165" s="0" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M166" s="0" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M167" s="0" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M168" s="0" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M169" s="0" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M170" s="0" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M171" s="0" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M172" s="0" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M173" s="0" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M174" s="0" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M175" s="0" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M176" s="0" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M177" s="0" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M178" s="0" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M179" s="0" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M180" s="0" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M181" s="0" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M182" s="0" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M183" s="0" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M184" s="0" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M185" s="0" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M186" s="0" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M187" s="0" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M188" s="0" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M189" s="0" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M190" s="0" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M191" s="0" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M192" s="0" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M193" s="0" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M194" s="0" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M195" s="0" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M196" s="0" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M197" s="0" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M198" s="0" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M199" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M200" s="0" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M201" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M202" s="0" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M203" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M204" s="0" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M205" s="0" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M206" s="0" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M207" s="0" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M208" s="0" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M209" s="0" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M210" s="0" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M211" s="0" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M212" s="0" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M213" s="0" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M214" s="0" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M215" s="0" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M216" s="0" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M217" s="0" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M218" s="0" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M219" s="0" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M220" s="0" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M221" s="0" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M222" s="0" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M223" s="0" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M224" s="0" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M225" s="0" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M226" s="0" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M227" s="0" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M228" s="0" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M229" s="0" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M230" s="0" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M231" s="0" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M232" s="0" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M233" s="0" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M234" s="0" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M235" s="0" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M236" s="0" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M237" s="0" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M238" s="0" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M239" s="0" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M240" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M241" s="0" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M242" s="0" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M243" s="0" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M244" s="0" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M245" s="0" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M246" s="0" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M247" s="0" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M248" s="0" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M249" s="0" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M250" s="0" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M251" s="0" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M252" s="0" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M253" s="0" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M254" s="0" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M255" s="0" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M256" s="0" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M257" s="0" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M258" s="0" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M259" s="0" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M260" s="0" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M261" s="0" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M262" s="0" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M263" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M264" s="0" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M265" s="0" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M266" s="0" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M267" s="0" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M268" s="0" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M269" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M270" s="0" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M271" s="0" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M272" s="0" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M273" s="0" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M274" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M275" s="0" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M276" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M277" s="0" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M278" s="0" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M279" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M280" s="0" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M281" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M282" s="0" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M283" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M284" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M285" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M286" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M287" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix + paired end xlsx example
</commit_message>
<xml_diff>
--- a/example_tables/ENA_excel_example_ERC000033.xlsx
+++ b/example_tables/ENA_excel_example_ERC000033.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="676">
   <si>
     <t xml:space="preserve">alias</t>
   </si>
@@ -776,9 +776,6 @@
   </si>
   <si>
     <t xml:space="preserve">ENA_TEST2.R1.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r_20221007_053</t>
   </si>
   <si>
     <t xml:space="preserve">ENA_TEST2.R2.fastq.gz</t>
@@ -2677,7 +2674,7 @@
   <dimension ref="A1:N101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4329,13 +4326,15 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="1" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="301" min="4" style="0" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4396,13 +4395,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>244</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>245</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>241</v>
@@ -4728,17 +4727,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4748,102 +4747,102 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4864,7 +4863,7 @@
   </sheetPr>
   <dimension ref="A1:AN101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -4881,118 +4880,118 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5000,121 +4999,121 @@
         <v>235</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5122,19 +5121,19 @@
         <v>56</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5143,34 +5142,34 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P3" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="S3" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="T3" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>50</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="W3" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="Y3" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="AA3" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AB3" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AG3" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="AG3" s="0" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,19 +5177,19 @@
         <v>66</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>43916</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5199,34 +5198,34 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P4" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="S4" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="S4" s="0" t="s">
-        <v>351</v>
-      </c>
       <c r="T4" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>46</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="W4" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="Y4" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="AA4" s="0" t="s">
         <v>354</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="AB4" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="AB4" s="0" t="s">
-        <v>356</v>
-      </c>
       <c r="AG4" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,19 +5233,19 @@
         <v>68</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L5" s="4" t="n">
         <v>43916</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5255,34 +5254,34 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P5" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="S5" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="S5" s="0" t="s">
-        <v>351</v>
-      </c>
       <c r="T5" s="0" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="U5" s="0" t="n">
         <v>70</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="W5" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="AG5" s="0" t="s">
         <v>363</v>
-      </c>
-      <c r="Y5" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="AA5" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="AB5" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="AG5" s="0" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5290,19 +5289,19 @@
         <v>70</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2697049</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L6" s="4" t="n">
         <v>43916</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>58.9276349289446</v>
@@ -5311,31 +5310,31 @@
         <v>25.2684466379874</v>
       </c>
       <c r="P6" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="S6" s="0" t="s">
-        <v>351</v>
-      </c>
       <c r="T6" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="AG6" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y6" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="AA6" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="AB6" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="AG6" s="0" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5873,74 +5872,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I1" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="M1" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>370</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="W1" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="AI1" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="W1" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AM1" s="0" t="s">
         <v>373</v>
-      </c>
-      <c r="AM1" s="0" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I2" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="M2" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>379</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="AI2" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="AI2" s="0" t="s">
+      <c r="AM2" s="0" t="s">
         <v>381</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M3" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="W3" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="AI3" s="0" t="s">
         <v>386</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>387</v>
       </c>
       <c r="AM3" s="0" t="s">
         <v>176</v>
@@ -5948,36 +5947,36 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M4" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q4" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="V4" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="W4" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="AI4" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="W4" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="AI4" s="0" t="s">
+      <c r="AM4" s="0" t="s">
         <v>391</v>
-      </c>
-      <c r="AM4" s="0" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M5" s="0" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q5" s="0" t="s">
         <v>176</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AI5" s="0" t="s">
         <v>176</v>
@@ -5985,126 +5984,126 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M6" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q6" s="0" t="s">
         <v>395</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="V6" s="0" t="s">
         <v>396</v>
       </c>
-      <c r="V6" s="0" t="s">
+      <c r="W6" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="AI6" s="0" t="s">
         <v>397</v>
-      </c>
-      <c r="W6" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="AI6" s="0" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M7" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="V7" s="0" t="s">
         <v>400</v>
       </c>
-      <c r="V7" s="0" t="s">
+      <c r="W7" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="AI7" s="0" t="s">
         <v>401</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="AI7" s="0" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M8" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="V8" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="V8" s="0" t="s">
-        <v>404</v>
-      </c>
       <c r="W8" s="0" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M9" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="V9" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="V9" s="0" t="s">
-        <v>406</v>
-      </c>
       <c r="W9" s="0" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M10" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="V10" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="V10" s="0" t="s">
-        <v>408</v>
-      </c>
       <c r="W10" s="0" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M11" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="V11" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="V11" s="0" t="s">
-        <v>410</v>
-      </c>
       <c r="W11" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M12" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="V12" s="0" t="s">
         <v>411</v>
       </c>
-      <c r="V12" s="0" t="s">
+      <c r="W12" s="0" t="s">
         <v>412</v>
-      </c>
-      <c r="W12" s="0" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M13" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M14" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="V14" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="V14" s="0" t="s">
-        <v>416</v>
-      </c>
       <c r="W14" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M15" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M16" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="W16" s="0" t="s">
         <v>176</v>
@@ -6112,1360 +6111,1360 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M17" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M18" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M19" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M20" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M21" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M22" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M23" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M24" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M25" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M26" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M27" s="0" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M28" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M29" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M30" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M31" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M32" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M33" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M34" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M35" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M36" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M37" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M38" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M39" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M40" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M41" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M42" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M43" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M44" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M45" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M46" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M47" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M48" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M49" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M50" s="0" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M51" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M52" s="0" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M53" s="0" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M54" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M55" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M56" s="0" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M57" s="0" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M58" s="0" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M59" s="0" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M60" s="0" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M61" s="0" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M62" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M63" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M64" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M65" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M66" s="0" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M67" s="0" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M68" s="0" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M69" s="0" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M70" s="0" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M71" s="0" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M72" s="0" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M73" s="0" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M74" s="0" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M75" s="0" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M76" s="0" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M77" s="0" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M78" s="0" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M79" s="0" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M80" s="0" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M81" s="0" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M82" s="0" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M83" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M84" s="0" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M85" s="0" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M86" s="0" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M87" s="0" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M88" s="0" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M89" s="0" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M90" s="0" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M91" s="0" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M92" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M93" s="0" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M94" s="0" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M95" s="0" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M96" s="0" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M97" s="0" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M98" s="0" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M99" s="0" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M100" s="0" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M101" s="0" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M102" s="0" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M103" s="0" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M104" s="0" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M105" s="0" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M106" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M107" s="0" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M108" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M109" s="0" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M110" s="0" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M111" s="0" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M112" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M113" s="0" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M114" s="0" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M115" s="0" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M116" s="0" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M117" s="0" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M118" s="0" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M119" s="0" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M120" s="0" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M121" s="0" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M122" s="0" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M123" s="0" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M124" s="0" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M125" s="0" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M126" s="0" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M127" s="0" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M128" s="0" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M129" s="0" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M130" s="0" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M131" s="0" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M132" s="0" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M133" s="0" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M134" s="0" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M135" s="0" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M136" s="0" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M137" s="0" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M138" s="0" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M139" s="0" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M140" s="0" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M141" s="0" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M142" s="0" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M143" s="0" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M144" s="0" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M145" s="0" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M146" s="0" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M147" s="0" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M148" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M149" s="0" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M150" s="0" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M151" s="0" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M152" s="0" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M153" s="0" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M154" s="0" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M155" s="0" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M156" s="0" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M157" s="0" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M158" s="0" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M159" s="0" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M160" s="0" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M161" s="0" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M162" s="0" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M163" s="0" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M164" s="0" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M165" s="0" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M166" s="0" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M167" s="0" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M168" s="0" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M169" s="0" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M170" s="0" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M171" s="0" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M172" s="0" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M173" s="0" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M174" s="0" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M175" s="0" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M176" s="0" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M177" s="0" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M178" s="0" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M179" s="0" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M180" s="0" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M181" s="0" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M182" s="0" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M183" s="0" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M184" s="0" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M185" s="0" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M186" s="0" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M187" s="0" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M188" s="0" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M189" s="0" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M190" s="0" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M191" s="0" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M192" s="0" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M193" s="0" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M194" s="0" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M195" s="0" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M196" s="0" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M197" s="0" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M198" s="0" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M199" s="0" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M200" s="0" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M201" s="0" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M202" s="0" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M203" s="0" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M204" s="0" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M205" s="0" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M206" s="0" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M207" s="0" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M208" s="0" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M209" s="0" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M210" s="0" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M211" s="0" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M212" s="0" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M213" s="0" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M214" s="0" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M215" s="0" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M216" s="0" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M217" s="0" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M218" s="0" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M219" s="0" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M220" s="0" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M221" s="0" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M222" s="0" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M223" s="0" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M224" s="0" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M225" s="0" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M226" s="0" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M227" s="0" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M228" s="0" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M229" s="0" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M230" s="0" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M231" s="0" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M232" s="0" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M233" s="0" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M234" s="0" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M235" s="0" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M236" s="0" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M237" s="0" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M238" s="0" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M239" s="0" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M240" s="0" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M241" s="0" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M242" s="0" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M243" s="0" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M244" s="0" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M245" s="0" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M246" s="0" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M247" s="0" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M248" s="0" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M249" s="0" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M250" s="0" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M251" s="0" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M252" s="0" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M253" s="0" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M254" s="0" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M255" s="0" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M256" s="0" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M257" s="0" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M258" s="0" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M259" s="0" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M260" s="0" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M261" s="0" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M262" s="0" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M263" s="0" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M264" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M265" s="0" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M266" s="0" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M267" s="0" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M268" s="0" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M269" s="0" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M270" s="0" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M271" s="0" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M272" s="0" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M273" s="0" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M274" s="0" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M275" s="0" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M276" s="0" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M277" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M278" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M279" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M280" s="0" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M281" s="0" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M282" s="0" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M283" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M284" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M285" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M286" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M287" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>